<commit_message>
Everything working, more refined
</commit_message>
<xml_diff>
--- a/excel_files/SLA_info.xlsx
+++ b/excel_files/SLA_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Created as Case Accepted</t>
+  </si>
+  <si>
+    <t>Flagged: Low risk but took less than 1 month.</t>
   </si>
 </sst>
 </file>
@@ -387,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,7 +409,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2">
-        <v>45292</v>
+        <v>45444</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -417,18 +420,18 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2">
-        <v>45323</v>
+        <v>45444</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2">
-        <v>45352</v>
+        <v>45474</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -439,10 +442,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2">
-        <v>45383</v>
+        <v>45474</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -450,7 +453,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2">
-        <v>45413</v>
+        <v>45505</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -461,78 +464,34 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2">
-        <v>45444</v>
+        <v>45505</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2">
-        <v>45536</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2">
-        <v>45566</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2">
-        <v>45597</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
-        <v>45627</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13">
         <v>0</v>
       </c>
     </row>

</xml_diff>